<commit_message>
first full working app
</commit_message>
<xml_diff>
--- a/Assets/To Do list.xlsx
+++ b/Assets/To Do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Amit\Projects\Programing\TextMe\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5590BBDF-636B-49A2-B73F-CDD3BAE197FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4F0624-8AE1-4342-B539-B3CDA9BDA483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11550" yWindow="2475" windowWidth="17250" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>make more formulas and questions</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>side menu</t>
+  </si>
+  <si>
+    <t>Try again on question</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,6 +513,9 @@
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">

</xml_diff>

<commit_message>
added try againg, colors and choose questions pack menu
</commit_message>
<xml_diff>
--- a/Assets/To Do list.xlsx
+++ b/Assets/To Do list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Amit\Projects\Programing\TextMe\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4F0624-8AE1-4342-B539-B3CDA9BDA483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3153939B-8C2D-426A-8A6A-9AB7C22C3644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11550" yWindow="2475" windowWidth="17250" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>make more formulas and questions</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Try again on question</t>
+  </si>
+  <si>
+    <t>log out button</t>
+  </si>
+  <si>
+    <t>friends in the side menu</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +134,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -142,11 +160,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -166,8 +186,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{152F094E-9934-4017-A90F-4A79C6A525EC}" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6" xr:uid="{AABC1B37-6A50-48EA-8138-FDE7DAE221CA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{152F094E-9934-4017-A90F-4A79C6A525EC}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{AABC1B37-6A50-48EA-8138-FDE7DAE221CA}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D1C3FFEF-204E-457C-BD86-D6CF669C5883}" name="UI"/>
     <tableColumn id="2" xr3:uid="{2B939D78-1DA0-46BE-9F6E-829C9553B0D3}" name="programing"/>
@@ -442,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +503,7 @@
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -494,10 +514,10 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -505,7 +525,7 @@
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -513,13 +533,21 @@
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
questions added and bugs fixed
</commit_message>
<xml_diff>
--- a/Assets/To Do list.xlsx
+++ b/Assets/To Do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Amit\Projects\Programing\TextMe\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3153939B-8C2D-426A-8A6A-9AB7C22C3644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58144036-06C4-4485-B84F-7CC19B593F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
@@ -541,12 +541,12 @@
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a new question pack
</commit_message>
<xml_diff>
--- a/Assets/To Do list.xlsx
+++ b/Assets/To Do list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Amit\Projects\Programing\TextMe\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58144036-06C4-4485-B84F-7CC19B593F12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B1F8EB-5599-4770-B2AF-CA051E3496E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>make more formulas and questions</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>friends in the side menu</t>
+  </si>
+  <si>
+    <t>Make end screen to the qeustions packs</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +149,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -160,13 +169,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -465,14 +475,14 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -500,7 +510,7 @@
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -516,6 +526,9 @@
       </c>
       <c r="B3" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>6</v>

</xml_diff>